<commit_message>
code added for Leap year
</commit_message>
<xml_diff>
--- a/Program_List.xlsx
+++ b/Program_List.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\MCA files\cds\C-_Programs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A659F0C4-16AE-43D7-82FB-B9CFF7DBD869}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E104FBF0-B5EC-4C3F-8876-78CCBFE6C084}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="99" uniqueCount="53">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="148" uniqueCount="54">
   <si>
     <t>Title</t>
   </si>
@@ -193,6 +193,9 @@
   </si>
   <si>
     <t>Multipath inharitance</t>
+  </si>
+  <si>
+    <t>Written</t>
   </si>
 </sst>
 </file>
@@ -265,7 +268,59 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="37">
+  <dxfs count="10">
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color theme="1"/>
+      </font>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <font>
         <strike val="0"/>
@@ -332,326 +387,6 @@
       </font>
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
@@ -666,11 +401,12 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{3035E0D0-34C6-43E9-8280-7425BAB2E596}" name="Table1" displayName="Table1" ref="A1:C49" totalsRowShown="0" headerRowDxfId="4" dataDxfId="3">
-  <tableColumns count="3">
-    <tableColumn id="3" xr3:uid="{FCBB1FF7-A779-4909-A6E8-B6FB4F0CBF1D}" name="S.no," dataDxfId="2"/>
-    <tableColumn id="1" xr3:uid="{56448B55-73DB-4843-B7FE-612BA2B9F122}" name="Title" dataDxfId="1"/>
-    <tableColumn id="2" xr3:uid="{970BAA8F-D99D-4103-8EDB-16692723B305}" name="Status" dataDxfId="0"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{3035E0D0-34C6-43E9-8280-7425BAB2E596}" name="Table1" displayName="Table1" ref="A1:D49" totalsRowShown="0" headerRowDxfId="9" dataDxfId="8">
+  <tableColumns count="4">
+    <tableColumn id="3" xr3:uid="{FCBB1FF7-A779-4909-A6E8-B6FB4F0CBF1D}" name="S.no," dataDxfId="7"/>
+    <tableColumn id="1" xr3:uid="{56448B55-73DB-4843-B7FE-612BA2B9F122}" name="Title" dataDxfId="6"/>
+    <tableColumn id="2" xr3:uid="{970BAA8F-D99D-4103-8EDB-16692723B305}" name="Status" dataDxfId="5"/>
+    <tableColumn id="4" xr3:uid="{835F213D-5AB8-4A90-B77D-B40E0E0FEB5F}" name="Written" dataDxfId="2"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium13" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -939,10 +675,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C49"/>
+  <dimension ref="A1:D49"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="83" workbookViewId="0">
-      <selection activeCell="D8" sqref="D8"/>
+    <sheetView tabSelected="1" topLeftCell="A13" zoomScale="83" workbookViewId="0">
+      <selection activeCell="E16" sqref="E16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="55.88671875" defaultRowHeight="28.8" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -953,7 +689,7 @@
     <col min="4" max="16384" width="55.88671875" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" ht="28.8" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:4" ht="28.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>6</v>
       </c>
@@ -963,8 +699,11 @@
       <c r="C1" s="1" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="2" spans="1:3" ht="28.8" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="D1" s="1" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" ht="28.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="3">
         <v>1</v>
       </c>
@@ -974,8 +713,11 @@
       <c r="C2" s="2" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="3" spans="1:3" ht="28.8" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="D2" s="2" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" ht="28.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" s="3">
         <v>2</v>
       </c>
@@ -985,8 +727,11 @@
       <c r="C3" s="2" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="4" spans="1:3" ht="28.8" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="D3" s="2" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" ht="28.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4" s="3">
         <v>3</v>
       </c>
@@ -996,8 +741,11 @@
       <c r="C4" s="2" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="5" spans="1:3" ht="28.8" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="D4" s="2" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" ht="28.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A5" s="1">
         <v>4</v>
       </c>
@@ -1007,8 +755,11 @@
       <c r="C5" s="2" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="6" spans="1:3" ht="28.8" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="D5" s="2" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" ht="28.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A6" s="1">
         <v>5</v>
       </c>
@@ -1018,8 +769,11 @@
       <c r="C6" s="2" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="7" spans="1:3" ht="28.8" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="D6" s="2" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" ht="28.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A7" s="1">
         <v>6</v>
       </c>
@@ -1029,8 +783,11 @@
       <c r="C7" s="2" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="8" spans="1:3" ht="28.8" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="D7" s="2" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" ht="28.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A8" s="1">
         <v>7</v>
       </c>
@@ -1040,8 +797,11 @@
       <c r="C8" s="2" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="9" spans="1:3" ht="28.8" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="D8" s="2" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" ht="28.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A9" s="1">
         <v>8</v>
       </c>
@@ -1051,8 +811,11 @@
       <c r="C9" s="2" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="10" spans="1:3" ht="28.8" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="D9" s="2" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" ht="28.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A10" s="1">
         <v>9</v>
       </c>
@@ -1062,8 +825,11 @@
       <c r="C10" s="2" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="11" spans="1:3" ht="28.8" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="D10" s="2" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" ht="28.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A11" s="1">
         <v>10</v>
       </c>
@@ -1073,8 +839,11 @@
       <c r="C11" s="2" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="12" spans="1:3" ht="28.8" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="D11" s="2" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" ht="28.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A12" s="1">
         <v>11</v>
       </c>
@@ -1084,8 +853,11 @@
       <c r="C12" s="2" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="13" spans="1:3" ht="28.8" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="D12" s="2" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" ht="28.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A13" s="1">
         <v>12</v>
       </c>
@@ -1095,8 +867,11 @@
       <c r="C13" s="2" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="14" spans="1:3" ht="28.8" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="D13" s="2" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" ht="28.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A14" s="1">
         <v>13</v>
       </c>
@@ -1106,8 +881,11 @@
       <c r="C14" s="2" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="15" spans="1:3" ht="28.8" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="D14" s="2" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" ht="28.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A15" s="1">
         <v>14</v>
       </c>
@@ -1115,10 +893,13 @@
         <v>17</v>
       </c>
       <c r="C15" s="2" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="16" spans="1:3" ht="28.8" customHeight="1" x14ac:dyDescent="0.3">
+        <v>3</v>
+      </c>
+      <c r="D15" s="2" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" ht="28.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A16" s="1">
         <v>15</v>
       </c>
@@ -1126,10 +907,13 @@
         <v>19</v>
       </c>
       <c r="C16" s="2" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="17" spans="1:3" ht="28.8" customHeight="1" x14ac:dyDescent="0.3">
+        <v>3</v>
+      </c>
+      <c r="D16" s="2" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" ht="28.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A17" s="1">
         <v>16</v>
       </c>
@@ -1137,10 +921,13 @@
         <v>20</v>
       </c>
       <c r="C17" s="2" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="18" spans="1:3" ht="28.8" customHeight="1" x14ac:dyDescent="0.3">
+        <v>3</v>
+      </c>
+      <c r="D17" s="2" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" ht="28.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A18" s="1">
         <v>17</v>
       </c>
@@ -1148,10 +935,13 @@
         <v>21</v>
       </c>
       <c r="C18" s="2" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="19" spans="1:3" ht="28.8" customHeight="1" x14ac:dyDescent="0.3">
+        <v>3</v>
+      </c>
+      <c r="D18" s="2" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" ht="28.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A19" s="1">
         <v>18</v>
       </c>
@@ -1159,10 +949,13 @@
         <v>22</v>
       </c>
       <c r="C19" s="2" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="20" spans="1:3" ht="28.8" customHeight="1" x14ac:dyDescent="0.3">
+        <v>3</v>
+      </c>
+      <c r="D19" s="2" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" ht="28.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A20" s="1">
         <v>19</v>
       </c>
@@ -1172,8 +965,11 @@
       <c r="C20" s="2" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="21" spans="1:3" ht="28.8" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="D20" s="2" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" ht="28.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A21" s="1">
         <v>20</v>
       </c>
@@ -1183,8 +979,11 @@
       <c r="C21" s="2" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="22" spans="1:3" ht="28.8" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="D21" s="2" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" ht="28.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A22" s="1">
         <v>21</v>
       </c>
@@ -1194,8 +993,11 @@
       <c r="C22" s="2" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="23" spans="1:3" ht="28.8" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="D22" s="2" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" ht="28.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A23" s="1">
         <v>22</v>
       </c>
@@ -1205,8 +1007,11 @@
       <c r="C23" s="2" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="24" spans="1:3" ht="28.8" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="D23" s="2" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" ht="28.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A24" s="1">
         <v>23</v>
       </c>
@@ -1216,8 +1021,11 @@
       <c r="C24" s="2" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="25" spans="1:3" ht="28.8" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="D24" s="2" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" ht="28.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A25" s="1">
         <v>24</v>
       </c>
@@ -1227,8 +1035,11 @@
       <c r="C25" s="2" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="26" spans="1:3" ht="28.8" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="D25" s="2" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" ht="28.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A26" s="1">
         <v>25</v>
       </c>
@@ -1238,8 +1049,11 @@
       <c r="C26" s="2" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="27" spans="1:3" ht="28.8" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="D26" s="2" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" ht="28.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A27" s="1">
         <v>26</v>
       </c>
@@ -1249,8 +1063,11 @@
       <c r="C27" s="2" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="28" spans="1:3" ht="28.8" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="D27" s="2" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4" ht="28.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A28" s="1">
         <v>27</v>
       </c>
@@ -1260,8 +1077,11 @@
       <c r="C28" s="2" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="29" spans="1:3" ht="28.8" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="D28" s="2" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4" ht="28.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A29" s="1">
         <v>28</v>
       </c>
@@ -1271,8 +1091,11 @@
       <c r="C29" s="2" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="30" spans="1:3" ht="28.8" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="D29" s="2" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4" ht="28.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A30" s="1">
         <v>29</v>
       </c>
@@ -1282,8 +1105,11 @@
       <c r="C30" s="2" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="31" spans="1:3" ht="28.8" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="D30" s="2" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4" ht="28.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A31" s="1">
         <v>30</v>
       </c>
@@ -1293,8 +1119,11 @@
       <c r="C31" s="2" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="32" spans="1:3" ht="28.8" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="D31" s="2" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="32" spans="1:4" ht="28.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A32" s="1">
         <v>31</v>
       </c>
@@ -1304,8 +1133,11 @@
       <c r="C32" s="2" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="33" spans="1:3" ht="28.8" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="D32" s="2" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="33" spans="1:4" ht="28.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A33" s="1">
         <v>32</v>
       </c>
@@ -1315,8 +1147,11 @@
       <c r="C33" s="2" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="34" spans="1:3" ht="28.8" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="D33" s="2" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="34" spans="1:4" ht="28.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A34" s="1">
         <v>33</v>
       </c>
@@ -1326,8 +1161,11 @@
       <c r="C34" s="2" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="35" spans="1:3" ht="28.8" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="D34" s="2" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="35" spans="1:4" ht="28.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A35" s="1">
         <v>34</v>
       </c>
@@ -1337,8 +1175,11 @@
       <c r="C35" s="2" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="36" spans="1:3" ht="28.8" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="D35" s="2" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="36" spans="1:4" ht="28.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A36" s="1">
         <v>35</v>
       </c>
@@ -1348,8 +1189,11 @@
       <c r="C36" s="2" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="37" spans="1:3" ht="28.8" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="D36" s="2" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="37" spans="1:4" ht="28.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A37" s="1">
         <v>36</v>
       </c>
@@ -1359,8 +1203,11 @@
       <c r="C37" s="2" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="38" spans="1:3" ht="28.8" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="D37" s="2" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="38" spans="1:4" ht="28.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A38" s="1">
         <v>37</v>
       </c>
@@ -1370,8 +1217,11 @@
       <c r="C38" s="2" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="39" spans="1:3" ht="28.8" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="D38" s="2" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="39" spans="1:4" ht="28.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A39" s="1">
         <v>38</v>
       </c>
@@ -1381,8 +1231,11 @@
       <c r="C39" s="2" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="40" spans="1:3" ht="28.8" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="D39" s="2" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="40" spans="1:4" ht="28.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A40" s="1">
         <v>39</v>
       </c>
@@ -1392,8 +1245,11 @@
       <c r="C40" s="2" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="41" spans="1:3" ht="28.8" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="D40" s="2" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="41" spans="1:4" ht="28.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A41" s="1">
         <v>40</v>
       </c>
@@ -1403,8 +1259,11 @@
       <c r="C41" s="2" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="42" spans="1:3" ht="28.8" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="D41" s="2" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="42" spans="1:4" ht="28.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A42" s="1">
         <v>41</v>
       </c>
@@ -1414,8 +1273,11 @@
       <c r="C42" s="2" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="43" spans="1:3" ht="28.8" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="D42" s="2" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="43" spans="1:4" ht="28.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A43" s="1">
         <v>42</v>
       </c>
@@ -1425,8 +1287,11 @@
       <c r="C43" s="2" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="44" spans="1:3" ht="28.8" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="D43" s="2" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="44" spans="1:4" ht="28.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A44" s="1">
         <v>43</v>
       </c>
@@ -1436,8 +1301,11 @@
       <c r="C44" s="2" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="45" spans="1:3" ht="28.8" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="D44" s="2" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="45" spans="1:4" ht="28.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A45" s="1">
         <v>44</v>
       </c>
@@ -1447,8 +1315,11 @@
       <c r="C45" s="2" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="46" spans="1:3" ht="28.8" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="D45" s="2" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="46" spans="1:4" ht="28.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A46" s="1">
         <v>45</v>
       </c>
@@ -1458,8 +1329,11 @@
       <c r="C46" s="2" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="47" spans="1:3" ht="28.8" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="D46" s="2" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="47" spans="1:4" ht="28.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A47" s="1">
         <v>46</v>
       </c>
@@ -1469,8 +1343,11 @@
       <c r="C47" s="2" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="48" spans="1:3" ht="28.8" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="D47" s="2" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="48" spans="1:4" ht="28.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A48" s="1">
         <v>47</v>
       </c>
@@ -1480,8 +1357,11 @@
       <c r="C48" s="2" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="49" spans="1:3" ht="28.8" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="D48" s="2" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="49" spans="1:4" ht="28.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A49" s="1">
         <v>48</v>
       </c>
@@ -1491,13 +1371,24 @@
       <c r="C49" s="2" t="s">
         <v>18</v>
       </c>
+      <c r="D49" s="2" t="s">
+        <v>18</v>
+      </c>
     </row>
   </sheetData>
-  <conditionalFormatting sqref="B14:B42 C1:C42 B43:C43 B44:B1048576 C44:C49">
-    <cfRule type="cellIs" dxfId="6" priority="1" operator="equal">
+  <conditionalFormatting sqref="B14:B42 B43:C43 C44:C49 B44:B1048576 C1:C42">
+    <cfRule type="cellIs" dxfId="4" priority="3" operator="equal">
       <formula>"i"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="5" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="3" priority="4" operator="equal">
+      <formula>"p"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D2:D49">
+    <cfRule type="cellIs" dxfId="1" priority="1" operator="equal">
+      <formula>"i"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="0" priority="2" operator="equal">
       <formula>"p"</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>

<commit_message>
added code for complex number,function overloading,neon number,factorial,armstrong,digit sum,string to upper case
</commit_message>
<xml_diff>
--- a/Program_List.xlsx
+++ b/Program_List.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\MCA files\cds\C-_Programs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E104FBF0-B5EC-4C3F-8876-78CCBFE6C084}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{539C3B0D-F577-40B1-8303-9D1AA400C925}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -120,15 +120,9 @@
     <t>Find min max among 3 number</t>
   </si>
   <si>
-    <t>Add complex number using frien function</t>
-  </si>
-  <si>
     <t>Function overloading</t>
   </si>
   <si>
-    <t>Check Nelson Number</t>
-  </si>
-  <si>
     <t>Factorial of a number using operator overloading</t>
   </si>
   <si>
@@ -196,6 +190,12 @@
   </si>
   <si>
     <t>Written</t>
+  </si>
+  <si>
+    <t>Add complex number using friend function</t>
+  </si>
+  <si>
+    <t>Check Neon Number</t>
   </si>
 </sst>
 </file>
@@ -291,18 +291,6 @@
     </dxf>
     <dxf>
       <font>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="12"/>
-        <color theme="1"/>
-      </font>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
         <color rgb="FF006100"/>
       </font>
       <fill>
@@ -320,6 +308,18 @@
           <bgColor rgb="FFFFC7CE"/>
         </patternFill>
       </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color theme="1"/>
+      </font>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
       <font>
@@ -406,7 +406,7 @@
     <tableColumn id="3" xr3:uid="{FCBB1FF7-A779-4909-A6E8-B6FB4F0CBF1D}" name="S.no," dataDxfId="7"/>
     <tableColumn id="1" xr3:uid="{56448B55-73DB-4843-B7FE-612BA2B9F122}" name="Title" dataDxfId="6"/>
     <tableColumn id="2" xr3:uid="{970BAA8F-D99D-4103-8EDB-16692723B305}" name="Status" dataDxfId="5"/>
-    <tableColumn id="4" xr3:uid="{835F213D-5AB8-4A90-B77D-B40E0E0FEB5F}" name="Written" dataDxfId="2"/>
+    <tableColumn id="4" xr3:uid="{835F213D-5AB8-4A90-B77D-B40E0E0FEB5F}" name="Written" dataDxfId="4"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium13" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -677,8 +677,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:D49"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" zoomScale="83" workbookViewId="0">
-      <selection activeCell="E16" sqref="E16"/>
+    <sheetView tabSelected="1" topLeftCell="A19" zoomScale="83" workbookViewId="0">
+      <selection activeCell="C32" sqref="C32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="55.88671875" defaultRowHeight="28.8" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -700,7 +700,7 @@
         <v>1</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
     </row>
     <row r="2" spans="1:4" ht="28.8" customHeight="1" x14ac:dyDescent="0.3">
@@ -963,7 +963,7 @@
         <v>23</v>
       </c>
       <c r="C20" s="2" t="s">
-        <v>18</v>
+        <v>3</v>
       </c>
       <c r="D20" s="2" t="s">
         <v>18</v>
@@ -977,7 +977,7 @@
         <v>24</v>
       </c>
       <c r="C21" s="2" t="s">
-        <v>18</v>
+        <v>3</v>
       </c>
       <c r="D21" s="2" t="s">
         <v>18</v>
@@ -991,7 +991,7 @@
         <v>25</v>
       </c>
       <c r="C22" s="2" t="s">
-        <v>18</v>
+        <v>3</v>
       </c>
       <c r="D22" s="2" t="s">
         <v>18</v>
@@ -1005,7 +1005,7 @@
         <v>26</v>
       </c>
       <c r="C23" s="2" t="s">
-        <v>18</v>
+        <v>3</v>
       </c>
       <c r="D23" s="2" t="s">
         <v>18</v>
@@ -1019,7 +1019,7 @@
         <v>27</v>
       </c>
       <c r="C24" s="2" t="s">
-        <v>18</v>
+        <v>3</v>
       </c>
       <c r="D24" s="2" t="s">
         <v>18</v>
@@ -1030,10 +1030,10 @@
         <v>24</v>
       </c>
       <c r="B25" s="4" t="s">
-        <v>28</v>
+        <v>52</v>
       </c>
       <c r="C25" s="2" t="s">
-        <v>18</v>
+        <v>3</v>
       </c>
       <c r="D25" s="2" t="s">
         <v>18</v>
@@ -1044,10 +1044,10 @@
         <v>25</v>
       </c>
       <c r="B26" s="4" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C26" s="2" t="s">
-        <v>18</v>
+        <v>3</v>
       </c>
       <c r="D26" s="2" t="s">
         <v>18</v>
@@ -1058,10 +1058,10 @@
         <v>26</v>
       </c>
       <c r="B27" s="4" t="s">
-        <v>30</v>
+        <v>53</v>
       </c>
       <c r="C27" s="2" t="s">
-        <v>18</v>
+        <v>3</v>
       </c>
       <c r="D27" s="2" t="s">
         <v>18</v>
@@ -1072,10 +1072,10 @@
         <v>27</v>
       </c>
       <c r="B28" s="4" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="C28" s="2" t="s">
-        <v>18</v>
+        <v>3</v>
       </c>
       <c r="D28" s="2" t="s">
         <v>18</v>
@@ -1086,10 +1086,10 @@
         <v>28</v>
       </c>
       <c r="B29" s="4" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="C29" s="2" t="s">
-        <v>18</v>
+        <v>3</v>
       </c>
       <c r="D29" s="2" t="s">
         <v>18</v>
@@ -1100,10 +1100,10 @@
         <v>29</v>
       </c>
       <c r="B30" s="4" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="C30" s="2" t="s">
-        <v>18</v>
+        <v>3</v>
       </c>
       <c r="D30" s="2" t="s">
         <v>18</v>
@@ -1114,10 +1114,10 @@
         <v>30</v>
       </c>
       <c r="B31" s="4" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="C31" s="2" t="s">
-        <v>18</v>
+        <v>3</v>
       </c>
       <c r="D31" s="2" t="s">
         <v>18</v>
@@ -1128,7 +1128,7 @@
         <v>31</v>
       </c>
       <c r="B32" s="4" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="C32" s="2" t="s">
         <v>18</v>
@@ -1142,7 +1142,7 @@
         <v>32</v>
       </c>
       <c r="B33" s="4" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="C33" s="2" t="s">
         <v>18</v>
@@ -1156,7 +1156,7 @@
         <v>33</v>
       </c>
       <c r="B34" s="4" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="C34" s="2" t="s">
         <v>18</v>
@@ -1170,7 +1170,7 @@
         <v>34</v>
       </c>
       <c r="B35" s="4" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="C35" s="2" t="s">
         <v>18</v>
@@ -1184,7 +1184,7 @@
         <v>35</v>
       </c>
       <c r="B36" s="4" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="C36" s="2" t="s">
         <v>18</v>
@@ -1198,7 +1198,7 @@
         <v>36</v>
       </c>
       <c r="B37" s="4" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="C37" s="2" t="s">
         <v>18</v>
@@ -1212,7 +1212,7 @@
         <v>37</v>
       </c>
       <c r="B38" s="4" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="C38" s="2" t="s">
         <v>18</v>
@@ -1226,7 +1226,7 @@
         <v>38</v>
       </c>
       <c r="B39" s="4" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="C39" s="2" t="s">
         <v>18</v>
@@ -1240,7 +1240,7 @@
         <v>39</v>
       </c>
       <c r="B40" s="4" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="C40" s="2" t="s">
         <v>18</v>
@@ -1254,7 +1254,7 @@
         <v>40</v>
       </c>
       <c r="B41" s="4" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="C41" s="2" t="s">
         <v>18</v>
@@ -1268,7 +1268,7 @@
         <v>41</v>
       </c>
       <c r="B42" s="4" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="C42" s="2" t="s">
         <v>18</v>
@@ -1282,7 +1282,7 @@
         <v>42</v>
       </c>
       <c r="B43" s="4" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="C43" s="2" t="s">
         <v>18</v>
@@ -1296,7 +1296,7 @@
         <v>43</v>
       </c>
       <c r="B44" s="4" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="C44" s="2" t="s">
         <v>18</v>
@@ -1310,7 +1310,7 @@
         <v>44</v>
       </c>
       <c r="B45" s="4" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="C45" s="2" t="s">
         <v>18</v>
@@ -1324,7 +1324,7 @@
         <v>45</v>
       </c>
       <c r="B46" s="4" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="C46" s="2" t="s">
         <v>18</v>
@@ -1338,7 +1338,7 @@
         <v>46</v>
       </c>
       <c r="B47" s="4" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="C47" s="2" t="s">
         <v>18</v>
@@ -1352,7 +1352,7 @@
         <v>47</v>
       </c>
       <c r="B48" s="4" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="C48" s="2" t="s">
         <v>18</v>
@@ -1366,7 +1366,7 @@
         <v>48</v>
       </c>
       <c r="B49" s="4" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="C49" s="2" t="s">
         <v>18</v>
@@ -1376,11 +1376,11 @@
       </c>
     </row>
   </sheetData>
-  <conditionalFormatting sqref="B14:B42 B43:C43 C44:C49 B44:B1048576 C1:C42">
-    <cfRule type="cellIs" dxfId="4" priority="3" operator="equal">
+  <conditionalFormatting sqref="C1:C42 B14:B42 B43:C43 C44:C49 B44:B1048576">
+    <cfRule type="cellIs" dxfId="3" priority="3" operator="equal">
       <formula>"i"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="3" priority="4" operator="equal">
+    <cfRule type="cellIs" dxfId="2" priority="4" operator="equal">
       <formula>"p"</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>

<commit_message>
added code for Diffrence of two dates,Pramid pattern,Programm to sort numbers (Bubble sort),Programm to sort names,Program of Matrix 2D array
</commit_message>
<xml_diff>
--- a/Program_List.xlsx
+++ b/Program_List.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\MCA files\cds\C-_Programs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{539C3B0D-F577-40B1-8303-9D1AA400C925}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{944AD345-B78F-47C0-932E-3762AA783B0E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -268,27 +268,7 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="10">
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
+  <dxfs count="8">
     <dxf>
       <font>
         <color rgb="FF006100"/>
@@ -401,12 +381,12 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{3035E0D0-34C6-43E9-8280-7425BAB2E596}" name="Table1" displayName="Table1" ref="A1:D49" totalsRowShown="0" headerRowDxfId="9" dataDxfId="8">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{3035E0D0-34C6-43E9-8280-7425BAB2E596}" name="Table1" displayName="Table1" ref="A1:D49" totalsRowShown="0" headerRowDxfId="7" dataDxfId="6">
   <tableColumns count="4">
-    <tableColumn id="3" xr3:uid="{FCBB1FF7-A779-4909-A6E8-B6FB4F0CBF1D}" name="S.no," dataDxfId="7"/>
-    <tableColumn id="1" xr3:uid="{56448B55-73DB-4843-B7FE-612BA2B9F122}" name="Title" dataDxfId="6"/>
-    <tableColumn id="2" xr3:uid="{970BAA8F-D99D-4103-8EDB-16692723B305}" name="Status" dataDxfId="5"/>
-    <tableColumn id="4" xr3:uid="{835F213D-5AB8-4A90-B77D-B40E0E0FEB5F}" name="Written" dataDxfId="4"/>
+    <tableColumn id="3" xr3:uid="{FCBB1FF7-A779-4909-A6E8-B6FB4F0CBF1D}" name="S.no," dataDxfId="5"/>
+    <tableColumn id="1" xr3:uid="{56448B55-73DB-4843-B7FE-612BA2B9F122}" name="Title" dataDxfId="4"/>
+    <tableColumn id="2" xr3:uid="{970BAA8F-D99D-4103-8EDB-16692723B305}" name="Status" dataDxfId="3"/>
+    <tableColumn id="4" xr3:uid="{835F213D-5AB8-4A90-B77D-B40E0E0FEB5F}" name="Written" dataDxfId="2"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium13" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -677,8 +657,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:D49"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A19" zoomScale="83" workbookViewId="0">
-      <selection activeCell="C32" sqref="C32"/>
+    <sheetView tabSelected="1" topLeftCell="A27" zoomScale="83" workbookViewId="0">
+      <selection activeCell="B35" sqref="B35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="55.88671875" defaultRowHeight="28.8" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -1131,7 +1111,7 @@
         <v>33</v>
       </c>
       <c r="C32" s="2" t="s">
-        <v>18</v>
+        <v>3</v>
       </c>
       <c r="D32" s="2" t="s">
         <v>18</v>
@@ -1145,7 +1125,7 @@
         <v>34</v>
       </c>
       <c r="C33" s="2" t="s">
-        <v>18</v>
+        <v>3</v>
       </c>
       <c r="D33" s="2" t="s">
         <v>18</v>
@@ -1156,10 +1136,10 @@
         <v>33</v>
       </c>
       <c r="B34" s="4" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="C34" s="2" t="s">
-        <v>18</v>
+        <v>3</v>
       </c>
       <c r="D34" s="2" t="s">
         <v>18</v>
@@ -1170,10 +1150,10 @@
         <v>34</v>
       </c>
       <c r="B35" s="4" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C35" s="2" t="s">
-        <v>18</v>
+        <v>3</v>
       </c>
       <c r="D35" s="2" t="s">
         <v>18</v>
@@ -1376,19 +1356,11 @@
       </c>
     </row>
   </sheetData>
-  <conditionalFormatting sqref="C1:C42 B14:B42 B43:C43 C44:C49 B44:B1048576">
-    <cfRule type="cellIs" dxfId="3" priority="3" operator="equal">
+  <conditionalFormatting sqref="C44:C49 B44:B1048576 C1:C35 B36:C43 B14:B35 D2:D49">
+    <cfRule type="cellIs" dxfId="1" priority="3" operator="equal">
       <formula>"i"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="2" priority="4" operator="equal">
-      <formula>"p"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D2:D49">
-    <cfRule type="cellIs" dxfId="1" priority="1" operator="equal">
-      <formula>"i"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="0" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="0" priority="4" operator="equal">
       <formula>"p"</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>

<commit_message>
added code 49 to 55
</commit_message>
<xml_diff>
--- a/Program_List.xlsx
+++ b/Program_List.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\MCA files\cds\C-_Programs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{727B6691-2D22-4002-BBBF-5F2705693F2C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{04131D8F-E5C0-49BB-AACD-F176D1BAB95D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="148" uniqueCount="54">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="184" uniqueCount="66">
   <si>
     <t>Title</t>
   </si>
@@ -196,6 +196,42 @@
   </si>
   <si>
     <t>Check Neon Number</t>
+  </si>
+  <si>
+    <t>Copy constructor</t>
+  </si>
+  <si>
+    <t>Decimal to binary conversion</t>
+  </si>
+  <si>
+    <t>Nelson Number (111,222,333)</t>
+  </si>
+  <si>
+    <t>Operater overloading usind friend function</t>
+  </si>
+  <si>
+    <t>Find the day from date of birth</t>
+  </si>
+  <si>
+    <t>Matrix Row and column sum program</t>
+  </si>
+  <si>
+    <t>String Function -&gt; user defined strlen,strcpy,strcat,strcmp</t>
+  </si>
+  <si>
+    <t>1D array ( INSERTION,DELETION,TRAVERSAL)</t>
+  </si>
+  <si>
+    <t>QUEUE ( INSERTION,DELETION,TRAVERSAL)</t>
+  </si>
+  <si>
+    <t>STACK ( INSERTION,DELETION,TRAVERSAL)</t>
+  </si>
+  <si>
+    <t>LINKED LIST ( INSERTION,DELETION,TRAVERSAL)</t>
+  </si>
+  <si>
+    <t>TREE ( INSERTION,DELETION,TRAVERSAL)</t>
   </si>
 </sst>
 </file>
@@ -268,7 +304,27 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="8">
+  <dxfs count="10">
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <font>
         <color rgb="FF006100"/>
@@ -381,12 +437,12 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{3035E0D0-34C6-43E9-8280-7425BAB2E596}" name="Table1" displayName="Table1" ref="A1:D49" totalsRowShown="0" headerRowDxfId="7" dataDxfId="6">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{3035E0D0-34C6-43E9-8280-7425BAB2E596}" name="Table1" displayName="Table1" ref="A1:D61" totalsRowShown="0" headerRowDxfId="9" dataDxfId="8">
   <tableColumns count="4">
-    <tableColumn id="3" xr3:uid="{FCBB1FF7-A779-4909-A6E8-B6FB4F0CBF1D}" name="S.no," dataDxfId="5"/>
-    <tableColumn id="1" xr3:uid="{56448B55-73DB-4843-B7FE-612BA2B9F122}" name="Title" dataDxfId="4"/>
-    <tableColumn id="2" xr3:uid="{970BAA8F-D99D-4103-8EDB-16692723B305}" name="Status" dataDxfId="3"/>
-    <tableColumn id="4" xr3:uid="{835F213D-5AB8-4A90-B77D-B40E0E0FEB5F}" name="Written" dataDxfId="2"/>
+    <tableColumn id="3" xr3:uid="{FCBB1FF7-A779-4909-A6E8-B6FB4F0CBF1D}" name="S.no," dataDxfId="7"/>
+    <tableColumn id="1" xr3:uid="{56448B55-73DB-4843-B7FE-612BA2B9F122}" name="Title" dataDxfId="6"/>
+    <tableColumn id="2" xr3:uid="{970BAA8F-D99D-4103-8EDB-16692723B305}" name="Status" dataDxfId="5"/>
+    <tableColumn id="4" xr3:uid="{835F213D-5AB8-4A90-B77D-B40E0E0FEB5F}" name="Written" dataDxfId="4"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium13" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -655,10 +711,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D49"/>
+  <sheetPr>
+    <pageSetUpPr fitToPage="1"/>
+  </sheetPr>
+  <dimension ref="A1:D61"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A40" zoomScale="83" workbookViewId="0">
-      <selection activeCell="C50" sqref="C50"/>
+    <sheetView tabSelected="1" topLeftCell="A51" zoomScale="83" workbookViewId="0">
+      <selection activeCell="B57" sqref="B57"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="55.88671875" defaultRowHeight="28.8" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -876,7 +935,7 @@
         <v>3</v>
       </c>
       <c r="D15" s="2" t="s">
-        <v>18</v>
+        <v>3</v>
       </c>
     </row>
     <row r="16" spans="1:4" ht="28.8" customHeight="1" x14ac:dyDescent="0.3">
@@ -890,7 +949,7 @@
         <v>3</v>
       </c>
       <c r="D16" s="2" t="s">
-        <v>18</v>
+        <v>3</v>
       </c>
     </row>
     <row r="17" spans="1:4" ht="28.8" customHeight="1" x14ac:dyDescent="0.3">
@@ -904,7 +963,7 @@
         <v>3</v>
       </c>
       <c r="D17" s="2" t="s">
-        <v>18</v>
+        <v>3</v>
       </c>
     </row>
     <row r="18" spans="1:4" ht="28.8" customHeight="1" x14ac:dyDescent="0.3">
@@ -918,7 +977,7 @@
         <v>3</v>
       </c>
       <c r="D18" s="2" t="s">
-        <v>18</v>
+        <v>3</v>
       </c>
     </row>
     <row r="19" spans="1:4" ht="28.8" customHeight="1" x14ac:dyDescent="0.3">
@@ -932,7 +991,7 @@
         <v>3</v>
       </c>
       <c r="D19" s="2" t="s">
-        <v>18</v>
+        <v>3</v>
       </c>
     </row>
     <row r="20" spans="1:4" ht="28.8" customHeight="1" x14ac:dyDescent="0.3">
@@ -1355,8 +1414,176 @@
         <v>18</v>
       </c>
     </row>
+    <row r="50" spans="1:4" ht="28.8" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A50" s="1">
+        <v>49</v>
+      </c>
+      <c r="B50" s="4" t="s">
+        <v>54</v>
+      </c>
+      <c r="C50" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="D50" s="2" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="51" spans="1:4" ht="28.8" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A51" s="1">
+        <v>50</v>
+      </c>
+      <c r="B51" s="4" t="s">
+        <v>55</v>
+      </c>
+      <c r="C51" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="D51" s="2" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="52" spans="1:4" ht="28.8" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A52" s="1">
+        <v>51</v>
+      </c>
+      <c r="B52" s="4" t="s">
+        <v>56</v>
+      </c>
+      <c r="C52" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="D52" s="2" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="53" spans="1:4" ht="28.8" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A53" s="1">
+        <v>52</v>
+      </c>
+      <c r="B53" s="4" t="s">
+        <v>57</v>
+      </c>
+      <c r="C53" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="D53" s="2" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="54" spans="1:4" ht="28.8" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A54" s="1">
+        <v>53</v>
+      </c>
+      <c r="B54" s="4" t="s">
+        <v>58</v>
+      </c>
+      <c r="C54" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="D54" s="2" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="55" spans="1:4" ht="28.8" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A55" s="1">
+        <v>54</v>
+      </c>
+      <c r="B55" s="4" t="s">
+        <v>59</v>
+      </c>
+      <c r="C55" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="D55" s="2" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="56" spans="1:4" ht="28.8" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A56" s="1">
+        <v>55</v>
+      </c>
+      <c r="B56" s="4" t="s">
+        <v>60</v>
+      </c>
+      <c r="C56" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="D56" s="2" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="57" spans="1:4" ht="28.8" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A57" s="1">
+        <v>56</v>
+      </c>
+      <c r="B57" s="4" t="s">
+        <v>61</v>
+      </c>
+      <c r="C57" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="D57" s="2" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="58" spans="1:4" ht="28.8" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A58" s="1">
+        <v>57</v>
+      </c>
+      <c r="B58" s="4" t="s">
+        <v>62</v>
+      </c>
+      <c r="C58" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="D58" s="2" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="59" spans="1:4" ht="28.8" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A59" s="1">
+        <v>58</v>
+      </c>
+      <c r="B59" s="4" t="s">
+        <v>63</v>
+      </c>
+      <c r="C59" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="D59" s="2" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="60" spans="1:4" ht="28.8" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A60" s="1">
+        <v>59</v>
+      </c>
+      <c r="B60" s="4" t="s">
+        <v>64</v>
+      </c>
+      <c r="C60" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="D60" s="2" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="61" spans="1:4" ht="28.8" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A61" s="1">
+        <v>60</v>
+      </c>
+      <c r="B61" s="4" t="s">
+        <v>65</v>
+      </c>
+      <c r="C61" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="D61" s="2" t="s">
+        <v>18</v>
+      </c>
+    </row>
   </sheetData>
-  <conditionalFormatting sqref="C1:C35 D2:D49 B14:B35 B36:C43 C44:C49 B44:B1048576">
+  <conditionalFormatting sqref="C1:C35 B14:B35 B36:C43 B44:B1048576 C44:C61 D2:D61">
     <cfRule type="cellIs" dxfId="1" priority="3" operator="equal">
       <formula>"i"</formula>
     </cfRule>
@@ -1365,7 +1592,7 @@
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
+  <pageSetup scale="46" fitToHeight="0" orientation="portrait" r:id="rId1"/>
   <tableParts count="1">
     <tablePart r:id="rId2"/>
   </tableParts>

</xml_diff>

<commit_message>
added code upto 63
</commit_message>
<xml_diff>
--- a/Program_List.xlsx
+++ b/Program_List.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\MCA files\cds\C-_Programs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{834AA704-113B-4BF5-B5F8-94DEF7054577}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6E678C78-00D2-4F6B-A942-86341A09B151}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="184" uniqueCount="66">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="193" uniqueCount="69">
   <si>
     <t>Title</t>
   </si>
@@ -232,6 +232,15 @@
   </si>
   <si>
     <t>TREE ( INSERTION,DELETION,TRAVERSAL)</t>
+  </si>
+  <si>
+    <t>BUBBLE SORT</t>
+  </si>
+  <si>
+    <t>SELECTION SORT</t>
+  </si>
+  <si>
+    <t>QUICK SORT</t>
   </si>
 </sst>
 </file>
@@ -304,7 +313,67 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="8">
+  <dxfs count="14">
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <font>
         <color rgb="FF006100"/>
@@ -417,12 +486,12 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{3035E0D0-34C6-43E9-8280-7425BAB2E596}" name="Table1" displayName="Table1" ref="A1:D61" totalsRowShown="0" headerRowDxfId="7" dataDxfId="6">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{3035E0D0-34C6-43E9-8280-7425BAB2E596}" name="Table1" displayName="Table1" ref="A1:D64" totalsRowShown="0" headerRowDxfId="13" dataDxfId="12">
   <tableColumns count="4">
-    <tableColumn id="3" xr3:uid="{FCBB1FF7-A779-4909-A6E8-B6FB4F0CBF1D}" name="S.no," dataDxfId="5"/>
-    <tableColumn id="1" xr3:uid="{56448B55-73DB-4843-B7FE-612BA2B9F122}" name="Title" dataDxfId="4"/>
-    <tableColumn id="2" xr3:uid="{970BAA8F-D99D-4103-8EDB-16692723B305}" name="Status" dataDxfId="3"/>
-    <tableColumn id="4" xr3:uid="{835F213D-5AB8-4A90-B77D-B40E0E0FEB5F}" name="Written" dataDxfId="2"/>
+    <tableColumn id="3" xr3:uid="{FCBB1FF7-A779-4909-A6E8-B6FB4F0CBF1D}" name="S.no," dataDxfId="11"/>
+    <tableColumn id="1" xr3:uid="{56448B55-73DB-4843-B7FE-612BA2B9F122}" name="Title" dataDxfId="10"/>
+    <tableColumn id="2" xr3:uid="{970BAA8F-D99D-4103-8EDB-16692723B305}" name="Status" dataDxfId="9"/>
+    <tableColumn id="4" xr3:uid="{835F213D-5AB8-4A90-B77D-B40E0E0FEB5F}" name="Written" dataDxfId="8"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium13" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -694,10 +763,10 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:D61"/>
+  <dimension ref="A1:D64"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A53" zoomScale="83" workbookViewId="0">
-      <selection activeCell="C63" sqref="C63"/>
+    <sheetView tabSelected="1" topLeftCell="A20" zoomScale="83" workbookViewId="0">
+      <selection activeCell="D23" sqref="D23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="55.88671875" defaultRowHeight="28.8" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -985,7 +1054,7 @@
         <v>3</v>
       </c>
       <c r="D20" s="2" t="s">
-        <v>18</v>
+        <v>3</v>
       </c>
     </row>
     <row r="21" spans="1:4" ht="28.8" customHeight="1" x14ac:dyDescent="0.3">
@@ -999,7 +1068,7 @@
         <v>3</v>
       </c>
       <c r="D21" s="2" t="s">
-        <v>18</v>
+        <v>3</v>
       </c>
     </row>
     <row r="22" spans="1:4" ht="28.8" customHeight="1" x14ac:dyDescent="0.3">
@@ -1013,7 +1082,7 @@
         <v>3</v>
       </c>
       <c r="D22" s="2" t="s">
-        <v>18</v>
+        <v>3</v>
       </c>
     </row>
     <row r="23" spans="1:4" ht="28.8" customHeight="1" x14ac:dyDescent="0.3">
@@ -1562,12 +1631,54 @@
         <v>18</v>
       </c>
     </row>
+    <row r="62" spans="1:4" ht="28.8" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A62" s="1">
+        <v>61</v>
+      </c>
+      <c r="B62" s="4" t="s">
+        <v>66</v>
+      </c>
+      <c r="C62" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="D62" s="2" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="63" spans="1:4" ht="28.8" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A63" s="1">
+        <v>62</v>
+      </c>
+      <c r="B63" s="4" t="s">
+        <v>67</v>
+      </c>
+      <c r="C63" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="D63" s="2" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="64" spans="1:4" ht="28.8" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A64" s="1">
+        <v>63</v>
+      </c>
+      <c r="B64" s="4" t="s">
+        <v>68</v>
+      </c>
+      <c r="C64" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="D64" s="2" t="s">
+        <v>18</v>
+      </c>
+    </row>
   </sheetData>
-  <conditionalFormatting sqref="C1:C35 D2:D61 B14:B35 B36:C43 C44:C61 B44:B1048576">
-    <cfRule type="cellIs" dxfId="1" priority="3" operator="equal">
+  <conditionalFormatting sqref="C1:C35 B14:B35 B36:C43 B44:B1048576 C44:C64 D2:D64">
+    <cfRule type="cellIs" dxfId="7" priority="3" operator="equal">
       <formula>"i"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="0" priority="4" operator="equal">
+    <cfRule type="cellIs" dxfId="6" priority="4" operator="equal">
       <formula>"p"</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>